<commit_message>
reestablished Python 2.6 compatibility, config files for examples now don't have intel compilers enabled by default (so you can compile everything with PGI)
</commit_message>
<xml_diff>
--- a/results/particle_results.xlsx
+++ b/results/particle_results.xlsx
@@ -1018,7 +1018,7 @@
               <a:defRPr/>
             </a:pPr>
             <a:r>
-              <a:rPr lang="de-DE" baseline="0"/>
+              <a:rPr lang="de-DE"/>
               <a:t>Particle Push, 1 Core Westmere Xeon CPU </a:t>
             </a:r>
           </a:p>
@@ -1027,7 +1027,7 @@
               <a:defRPr/>
             </a:pPr>
             <a:r>
-              <a:rPr lang="de-DE" baseline="0"/>
+              <a:rPr lang="de-DE"/>
               <a:t>[Millions of Point Updates per Second]</a:t>
             </a:r>
           </a:p>
@@ -1172,11 +1172,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2103520504"/>
-        <c:axId val="-2103517320"/>
+        <c:axId val="2141703432"/>
+        <c:axId val="2141706520"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2103520504"/>
+        <c:axId val="2141703432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1186,17 +1186,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400"/>
-            </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="-2103517320"/>
+        <c:crossAx val="2141706520"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1204,7 +1194,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2103517320"/>
+        <c:axId val="2141706520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1215,7 +1205,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2103520504"/>
+        <c:crossAx val="2141703432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1224,6 +1214,16 @@
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1800"/>
+      </a:pPr>
+      <a:endParaRPr lang="de-DE"/>
+    </a:p>
+  </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
@@ -1256,18 +1256,8 @@
               <a:defRPr/>
             </a:pPr>
             <a:r>
-              <a:rPr lang="de-DE" sz="1800" b="1" i="0" u="none" strike="noStrike" baseline="0">
-                <a:effectLst/>
-              </a:rPr>
-              <a:t>Particle Push</a:t>
-            </a:r>
-            <a:r>
               <a:rPr lang="de-DE"/>
-              <a:t>,</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="de-DE" baseline="0"/>
-              <a:t> 6 Core Westmere Xeon CPU (1 Socket)</a:t>
+              <a:t>Particle Push, 6 Core Westmere Xeon CPU (1 Socket)</a:t>
             </a:r>
           </a:p>
           <a:p>
@@ -1275,14 +1265,9 @@
               <a:defRPr/>
             </a:pPr>
             <a:r>
-              <a:rPr lang="de-DE" sz="1800" b="1" i="0" baseline="0">
-                <a:effectLst/>
-              </a:rPr>
+              <a:rPr lang="de-DE"/>
               <a:t>[Millions of Point Updates per Second]</a:t>
             </a:r>
-            <a:endParaRPr lang="de-DE">
-              <a:effectLst/>
-            </a:endParaRPr>
           </a:p>
         </c:rich>
       </c:tx>
@@ -1465,11 +1450,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2104404232"/>
-        <c:axId val="2121359080"/>
+        <c:axId val="2141742408"/>
+        <c:axId val="2141745592"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2104404232"/>
+        <c:axId val="2141742408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1479,17 +1464,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400"/>
-            </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="2121359080"/>
+        <c:crossAx val="2141745592"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1497,7 +1472,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2121359080"/>
+        <c:axId val="2141745592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1508,7 +1483,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2104404232"/>
+        <c:crossAx val="2141742408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1517,6 +1492,16 @@
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1800"/>
+      </a:pPr>
+      <a:endParaRPr lang="de-DE"/>
+    </a:p>
+  </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
@@ -1558,14 +1543,9 @@
               <a:defRPr/>
             </a:pPr>
             <a:r>
-              <a:rPr lang="de-DE" sz="1800" b="1" i="0" baseline="0">
-                <a:effectLst/>
-              </a:rPr>
+              <a:rPr lang="de-DE"/>
               <a:t>[Millions of Point Updates per Second]</a:t>
             </a:r>
-            <a:endParaRPr lang="de-DE">
-              <a:effectLst/>
-            </a:endParaRPr>
           </a:p>
         </c:rich>
       </c:tx>
@@ -1724,11 +1704,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2122227928"/>
-        <c:axId val="2122151512"/>
+        <c:axId val="2141778760"/>
+        <c:axId val="2141781944"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2122227928"/>
+        <c:axId val="2141778760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1738,17 +1718,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400"/>
-            </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="2122151512"/>
+        <c:crossAx val="2141781944"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1756,7 +1726,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2122151512"/>
+        <c:axId val="2141781944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1767,7 +1737,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2122227928"/>
+        <c:crossAx val="2141778760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1776,6 +1746,16 @@
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1800"/>
+      </a:pPr>
+      <a:endParaRPr lang="de-DE"/>
+    </a:p>
+  </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
@@ -1982,11 +1962,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2074418552"/>
-        <c:axId val="2074421640"/>
+        <c:axId val="2141815544"/>
+        <c:axId val="2141818632"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2074418552"/>
+        <c:axId val="2141815544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2006,7 +1986,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2074421640"/>
+        <c:crossAx val="2141818632"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2014,7 +1994,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2074421640"/>
+        <c:axId val="2141818632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2025,7 +2005,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2074418552"/>
+        <c:crossAx val="2141815544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3564,8 +3544,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M45"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="B165" workbookViewId="0">
+      <selection activeCell="A122" sqref="A122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>